<commit_message>
MOS-23045: Update Master Data as per 22 April Changes
</commit_message>
<xml_diff>
--- a/docs/requirements/Master Data Tables - Test Data/master-applicant_valid_document.xlsx
+++ b/docs/requirements/Master Data Tables - Test Data/master-applicant_valid_document.xlsx
@@ -1,25 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1045476\Desktop\New folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\M1045452\Documents\GitHub\mosip\docs\requirements\Master Data Tables - Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21D6B5E9-D509-44F5-92A7-2A8FCACD11A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="master-valid_document" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'master-valid_document'!$A$1:$G$57</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="20">
   <si>
     <t>doctyp_code</t>
   </si>
@@ -84,7 +88,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000"/>
   </numFmts>
@@ -924,11 +928,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G57"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:G64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58:XFD1048576"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,25 +943,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2249,7 +2253,169 @@
         <v>9</v>
       </c>
     </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="3">
+        <v>3</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E58" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="3">
+        <v>4</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E59" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="3">
+        <v>7</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E60" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="3">
+        <v>8</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="3">
+        <v>11</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E62" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>12</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E63" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>15</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E64" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:G57" xr:uid="{14350AEC-E9D7-4943-9F1B-0F0B39D7E867}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>